<commit_message>
[CHANGED] renamed sheet to "Cards" and added category to xlsx file
</commit_message>
<xml_diff>
--- a/Data/GNH Card Data.xlsx
+++ b/Data/GNH Card Data.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cards" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -88,12 +88,6 @@
     <t>TreasuryL</t>
   </si>
   <si>
-    <t>RANDOM.1</t>
-  </si>
-  <si>
-    <t>EVENT1.1</t>
-  </si>
-  <si>
     <t>These cards will be in queue in a random order</t>
   </si>
   <si>
@@ -137,6 +131,15 @@
   </si>
   <si>
     <t>BackgroundColor</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Event1</t>
   </si>
 </sst>
 </file>
@@ -531,101 +534,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" t="s">
-        <v>21</v>
-      </c>
-      <c r="P1" t="s">
-        <v>20</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
       </c>
       <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
       <c r="E3">
         <v>1</v>
       </c>
@@ -639,7 +646,7 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>-1</v>
@@ -653,36 +660,39 @@
       <c r="M3">
         <v>-1</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <v>-1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>20</v>
+      </c>
+      <c r="P3" t="s">
         <v>22</v>
       </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="s">
-        <v>23</v>
+      <c r="Q3" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+      <c r="C4" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1100</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -697,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>-1</v>
@@ -711,14 +721,17 @@
       <c r="M5">
         <v>-1</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5">
+        <v>-1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>20</v>
+      </c>
+      <c r="P5" t="s">
         <v>22</v>
       </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="s">
-        <v>23</v>
+      <c r="Q5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[FIXED] several issues with parsing, array sizes, etc [CHANGED] imported card data to work with
</commit_message>
<xml_diff>
--- a/Data/GNH Card Data.xlsx
+++ b/Data/GNH Card Data.xlsx
@@ -364,10 +364,10 @@
     <t>Didn't think that day would come</t>
   </si>
   <si>
-    <t>Follow Up ID</t>
-  </si>
-  <si>
     <t>FollowUp</t>
+  </si>
+  <si>
+    <t>FollowUpId</t>
   </si>
 </sst>
 </file>
@@ -915,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -964,7 +964,7 @@
         <v>16</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>5</v>
@@ -1079,6 +1079,9 @@
       <c r="G3" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3" s="24">
         <v>15</v>
       </c>
@@ -1188,6 +1191,9 @@
       <c r="G5" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="H5" s="4">
+        <v>0</v>
+      </c>
       <c r="I5" s="24">
         <v>-10</v>
       </c>
@@ -1241,6 +1247,9 @@
       <c r="G6" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
       <c r="I6" s="24">
         <v>-5</v>
       </c>
@@ -1349,6 +1358,9 @@
       </c>
       <c r="G8" s="2" t="s">
         <v>70</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
       </c>
       <c r="I8" s="24">
         <v>10</v>
@@ -1463,6 +1475,9 @@
       <c r="G10" s="2" t="s">
         <v>76</v>
       </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
       <c r="I10" s="24">
         <v>0</v>
       </c>
@@ -1516,6 +1531,9 @@
       <c r="G11" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
       <c r="I11" s="24">
         <v>10</v>
       </c>
@@ -1569,6 +1587,9 @@
       <c r="G12" s="2" t="s">
         <v>82</v>
       </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
       <c r="I12" s="24">
         <v>0</v>
       </c>
@@ -1621,6 +1642,9 @@
       </c>
       <c r="G13" s="2" t="s">
         <v>85</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0</v>
       </c>
       <c r="I13" s="24">
         <v>0</v>
@@ -1735,6 +1759,9 @@
       <c r="G15" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
       <c r="I15" s="25">
         <v>5</v>
       </c>
@@ -1788,6 +1815,9 @@
       <c r="G16" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
       <c r="I16" s="25">
         <v>5</v>
       </c>
@@ -1841,6 +1871,9 @@
       <c r="G17" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="H17" s="4">
+        <v>0</v>
+      </c>
       <c r="I17" s="25">
         <v>0</v>
       </c>
@@ -1893,6 +1926,9 @@
       </c>
       <c r="G18" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0</v>
       </c>
       <c r="I18" s="25">
         <v>10</v>
@@ -2007,6 +2043,9 @@
       <c r="G20" s="3" t="s">
         <v>36</v>
       </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
       <c r="I20" s="25">
         <v>0</v>
       </c>
@@ -2060,6 +2099,9 @@
       <c r="G21" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
       <c r="I21" s="25">
         <v>5</v>
       </c>
@@ -2113,6 +2155,9 @@
       <c r="G22" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
       <c r="I22" s="25">
         <v>0</v>
       </c>
@@ -2166,6 +2211,9 @@
       <c r="G23" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
       <c r="I23" s="25">
         <v>0</v>
       </c>
@@ -2219,6 +2267,9 @@
       <c r="G24" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
       <c r="I24" s="25">
         <v>0</v>
       </c>
@@ -2271,6 +2322,9 @@
       </c>
       <c r="G25" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0</v>
       </c>
       <c r="I25" s="25">
         <v>10</v>
@@ -2368,7 +2422,7 @@
         <v>2000</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>89</v>
@@ -2384,6 +2438,9 @@
       </c>
       <c r="G27" s="2" t="s">
         <v>95</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0</v>
       </c>
       <c r="I27" s="4">
         <v>0</v>
@@ -2421,7 +2478,7 @@
         <v>2001</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>89</v>
@@ -2477,7 +2534,7 @@
         <v>2002</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>89</v>
@@ -2493,6 +2550,9 @@
       </c>
       <c r="G29" s="2" t="s">
         <v>101</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
       </c>
       <c r="I29" s="4">
         <v>10</v>

</xml_diff>

<commit_message>
[CHANGED] added follow up fields to data table and adjusted values
</commit_message>
<xml_diff>
--- a/Data/GNH Card Data.xlsx
+++ b/Data/GNH Card Data.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="108">
   <si>
     <t>ID</t>
   </si>
@@ -367,7 +367,16 @@
     <t>FollowUp</t>
   </si>
   <si>
-    <t>FollowUpId</t>
+    <t>FollowUpIdL</t>
+  </si>
+  <si>
+    <t>FollowUpIdR</t>
+  </si>
+  <si>
+    <t>FollowUpStepL</t>
+  </si>
+  <si>
+    <t>FollowUpStepR</t>
   </si>
 </sst>
 </file>
@@ -913,10 +922,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -927,21 +936,23 @@
     <col min="4" max="4" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.7109375" style="2" customWidth="1"/>
     <col min="6" max="7" width="20.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -966,38 +977,47 @@
       <c r="H1" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="R1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -1008,56 +1028,59 @@
       <c r="D2" s="11"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12">
-        <f>SUM(I2:M2)</f>
+        <f>SUM(L2:P2)</f>
         <v>0</v>
       </c>
       <c r="G2" s="12">
-        <f>SUM(N2:R2)</f>
+        <f>SUM(Q2:U2)</f>
         <v>-5</v>
       </c>
       <c r="H2" s="11"/>
-      <c r="I2" s="11">
-        <f>SUM(I3:I8)</f>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11">
+        <f>SUM(L3:L8)</f>
         <v>5</v>
       </c>
-      <c r="J2" s="11">
-        <f t="shared" ref="J2:R2" si="0">SUM(J3:J8)</f>
+      <c r="M2" s="11">
+        <f t="shared" ref="M2:U2" si="0">SUM(M3:M8)</f>
         <v>-5</v>
       </c>
-      <c r="K2" s="11">
+      <c r="N2" s="11">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="L2" s="11">
+      <c r="O2" s="11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="M2" s="11">
+      <c r="P2" s="11">
         <f t="shared" si="0"/>
         <v>-5</v>
       </c>
-      <c r="N2" s="11">
+      <c r="Q2" s="11">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="O2" s="11">
+      <c r="R2" s="11">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="P2" s="11">
+      <c r="S2" s="11">
         <f t="shared" si="0"/>
         <v>-15</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="T2" s="11">
         <f t="shared" si="0"/>
         <v>-10</v>
       </c>
-      <c r="R2" s="11">
+      <c r="U2" s="11">
         <f t="shared" si="0"/>
         <v>-45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>1000</v>
       </c>
@@ -1082,38 +1105,47 @@
       <c r="H3" s="4">
         <v>0</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0</v>
+      </c>
+      <c r="K3" s="4">
+        <v>0</v>
+      </c>
+      <c r="L3" s="24">
         <v>15</v>
       </c>
-      <c r="J3" s="24">
-        <v>-10</v>
-      </c>
-      <c r="K3" s="24">
+      <c r="M3" s="24">
+        <v>-10</v>
+      </c>
+      <c r="N3" s="24">
         <v>5</v>
       </c>
-      <c r="L3" s="24">
-        <v>0</v>
-      </c>
-      <c r="M3" s="24">
-        <v>-5</v>
-      </c>
-      <c r="N3" s="24">
-        <v>-15</v>
-      </c>
       <c r="O3" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P3" s="24">
         <v>-5</v>
       </c>
       <c r="Q3" s="24">
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="R3" s="24">
+        <v>10</v>
+      </c>
+      <c r="S3" s="24">
+        <v>-5</v>
+      </c>
+      <c r="T3" s="24">
+        <v>0</v>
+      </c>
+      <c r="U3" s="24">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>1001</v>
       </c>
@@ -1136,40 +1168,49 @@
         <v>59</v>
       </c>
       <c r="H4" s="4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="4">
         <v>2000</v>
       </c>
-      <c r="I4" s="24">
+      <c r="J4" s="4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="24">
         <v>-5</v>
       </c>
-      <c r="J4" s="24">
+      <c r="M4" s="24">
         <v>5</v>
       </c>
-      <c r="K4" s="24">
-        <v>0</v>
-      </c>
-      <c r="L4" s="24">
-        <v>0</v>
-      </c>
-      <c r="M4" s="24">
-        <v>0</v>
-      </c>
       <c r="N4" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O4" s="24">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="P4" s="24">
         <v>0</v>
       </c>
       <c r="Q4" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R4" s="24">
         <v>-10</v>
       </c>
+      <c r="S4" s="24">
+        <v>0</v>
+      </c>
+      <c r="T4" s="24">
+        <v>0</v>
+      </c>
+      <c r="U4" s="24">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>1002</v>
       </c>
@@ -1194,38 +1235,47 @@
       <c r="H5" s="4">
         <v>0</v>
       </c>
-      <c r="I5" s="24">
-        <v>-10</v>
-      </c>
-      <c r="J5" s="24">
-        <v>0</v>
-      </c>
-      <c r="K5" s="24">
+      <c r="I5" s="4">
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0</v>
+      </c>
+      <c r="K5" s="4">
         <v>0</v>
       </c>
       <c r="L5" s="24">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="M5" s="24">
         <v>0</v>
       </c>
       <c r="N5" s="24">
+        <v>0</v>
+      </c>
+      <c r="O5" s="24">
+        <v>0</v>
+      </c>
+      <c r="P5" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="24">
         <v>20</v>
       </c>
-      <c r="O5" s="24">
-        <v>10</v>
-      </c>
-      <c r="P5" s="24">
-        <v>-10</v>
-      </c>
-      <c r="Q5" s="24">
-        <v>-10</v>
-      </c>
       <c r="R5" s="24">
+        <v>10</v>
+      </c>
+      <c r="S5" s="24">
+        <v>-10</v>
+      </c>
+      <c r="T5" s="24">
+        <v>-10</v>
+      </c>
+      <c r="U5" s="24">
         <v>-15</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>1003</v>
       </c>
@@ -1250,38 +1300,47 @@
       <c r="H6" s="4">
         <v>0</v>
       </c>
-      <c r="I6" s="24">
+      <c r="I6" s="4">
+        <v>0</v>
+      </c>
+      <c r="J6" s="4">
+        <v>0</v>
+      </c>
+      <c r="K6" s="4">
+        <v>0</v>
+      </c>
+      <c r="L6" s="24">
         <v>-5</v>
       </c>
-      <c r="J6" s="24">
-        <v>0</v>
-      </c>
-      <c r="K6" s="24">
-        <v>0</v>
-      </c>
-      <c r="L6" s="24">
-        <v>0</v>
-      </c>
       <c r="M6" s="24">
         <v>0</v>
       </c>
       <c r="N6" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O6" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P6" s="24">
         <v>0</v>
       </c>
       <c r="Q6" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R6" s="24">
+        <v>10</v>
+      </c>
+      <c r="S6" s="24">
+        <v>0</v>
+      </c>
+      <c r="T6" s="24">
+        <v>0</v>
+      </c>
+      <c r="U6" s="24">
         <v>-10</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>1004</v>
       </c>
@@ -1304,15 +1363,15 @@
         <v>67</v>
       </c>
       <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4">
         <v>2001</v>
       </c>
-      <c r="I7" s="24">
-        <v>0</v>
-      </c>
-      <c r="J7" s="24">
-        <v>0</v>
-      </c>
-      <c r="K7" s="24">
+      <c r="J7" s="4">
+        <v>0</v>
+      </c>
+      <c r="K7" s="4">
         <v>0</v>
       </c>
       <c r="L7" s="24">
@@ -1325,7 +1384,7 @@
         <v>0</v>
       </c>
       <c r="O7" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P7" s="24">
         <v>0</v>
@@ -1334,10 +1393,19 @@
         <v>0</v>
       </c>
       <c r="R7" s="24">
+        <v>10</v>
+      </c>
+      <c r="S7" s="24">
+        <v>0</v>
+      </c>
+      <c r="T7" s="24">
+        <v>0</v>
+      </c>
+      <c r="U7" s="24">
         <v>-15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>1005</v>
       </c>
@@ -1362,23 +1430,23 @@
       <c r="H8" s="4">
         <v>0</v>
       </c>
-      <c r="I8" s="24">
-        <v>10</v>
-      </c>
-      <c r="J8" s="24">
-        <v>0</v>
-      </c>
-      <c r="K8" s="24">
+      <c r="I8" s="4">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0</v>
+      </c>
+      <c r="K8" s="4">
         <v>0</v>
       </c>
       <c r="L8" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M8" s="24">
         <v>0</v>
       </c>
       <c r="N8" s="24">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O8" s="24">
         <v>0</v>
@@ -1387,13 +1455,22 @@
         <v>0</v>
       </c>
       <c r="Q8" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R8" s="24">
         <v>0</v>
       </c>
+      <c r="S8" s="24">
+        <v>0</v>
+      </c>
+      <c r="T8" s="24">
+        <v>0</v>
+      </c>
+      <c r="U8" s="24">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:18" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>3</v>
       </c>
@@ -1404,56 +1481,59 @@
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18">
-        <f>SUM(I9:M9)</f>
+        <f>SUM(L9:P9)</f>
         <v>-15</v>
       </c>
       <c r="G9" s="18">
-        <f>SUM(N9:R9)</f>
+        <f>SUM(Q9:U9)</f>
         <v>5</v>
       </c>
       <c r="H9" s="17"/>
-      <c r="I9" s="17">
-        <f>SUM(I10:I13)</f>
-        <v>10</v>
-      </c>
-      <c r="J9" s="17">
-        <f t="shared" ref="J9:R9" si="1">SUM(J10:J13)</f>
-        <v>-10</v>
-      </c>
-      <c r="K9" s="17">
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17">
+        <f>SUM(L10:L13)</f>
+        <v>10</v>
+      </c>
+      <c r="M9" s="17">
+        <f t="shared" ref="M9:U9" si="1">SUM(M10:M13)</f>
+        <v>-10</v>
+      </c>
+      <c r="N9" s="17">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="L9" s="17">
+      <c r="O9" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M9" s="17">
+      <c r="P9" s="17">
         <f t="shared" si="1"/>
         <v>-5</v>
       </c>
-      <c r="N9" s="17">
+      <c r="Q9" s="17">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="O9" s="17">
+      <c r="R9" s="17">
         <f t="shared" si="1"/>
         <v>-20</v>
       </c>
-      <c r="P9" s="17">
+      <c r="S9" s="17">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="Q9" s="17">
+      <c r="T9" s="17">
         <f t="shared" si="1"/>
         <v>-10</v>
       </c>
-      <c r="R9" s="17">
+      <c r="U9" s="17">
         <f t="shared" si="1"/>
         <v>-15</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>1100</v>
       </c>
@@ -1478,38 +1558,47 @@
       <c r="H10" s="4">
         <v>0</v>
       </c>
-      <c r="I10" s="24">
-        <v>0</v>
-      </c>
-      <c r="J10" s="24">
-        <v>0</v>
-      </c>
-      <c r="K10" s="24">
+      <c r="I10" s="4">
+        <v>0</v>
+      </c>
+      <c r="J10" s="4">
+        <v>0</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24">
+        <v>0</v>
+      </c>
+      <c r="M10" s="24">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24">
         <v>-5</v>
       </c>
-      <c r="L10" s="24">
-        <v>0</v>
-      </c>
-      <c r="M10" s="24">
-        <v>0</v>
-      </c>
-      <c r="N10" s="24">
+      <c r="O10" s="24">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="24">
         <v>5</v>
       </c>
-      <c r="O10" s="24">
-        <v>-10</v>
-      </c>
-      <c r="P10" s="24">
-        <v>10</v>
-      </c>
-      <c r="Q10" s="24">
-        <v>0</v>
-      </c>
       <c r="R10" s="24">
+        <v>-10</v>
+      </c>
+      <c r="S10" s="24">
+        <v>10</v>
+      </c>
+      <c r="T10" s="24">
+        <v>0</v>
+      </c>
+      <c r="U10" s="24">
         <v>-5</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>1101</v>
       </c>
@@ -1534,38 +1623,47 @@
       <c r="H11" s="4">
         <v>0</v>
       </c>
-      <c r="I11" s="24">
-        <v>10</v>
-      </c>
-      <c r="J11" s="24">
-        <v>0</v>
-      </c>
-      <c r="K11" s="24">
-        <v>-10</v>
+      <c r="I11" s="4">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0</v>
       </c>
       <c r="L11" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M11" s="24">
         <v>0</v>
       </c>
       <c r="N11" s="24">
+        <v>-10</v>
+      </c>
+      <c r="O11" s="24">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="24">
         <v>-5</v>
       </c>
-      <c r="O11" s="24">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
+      <c r="R11" s="24">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24">
         <v>20</v>
       </c>
-      <c r="Q11" s="24">
-        <v>0</v>
-      </c>
-      <c r="R11" s="24">
+      <c r="T11" s="24">
+        <v>0</v>
+      </c>
+      <c r="U11" s="24">
         <v>-15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>1102</v>
       </c>
@@ -1590,38 +1688,47 @@
       <c r="H12" s="4">
         <v>0</v>
       </c>
-      <c r="I12" s="24">
-        <v>0</v>
-      </c>
-      <c r="J12" s="24">
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4">
+        <v>0</v>
+      </c>
+      <c r="K12" s="4">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24">
+        <v>0</v>
+      </c>
+      <c r="M12" s="24">
         <v>-20</v>
       </c>
-      <c r="K12" s="24">
+      <c r="N12" s="24">
         <v>15</v>
       </c>
-      <c r="L12" s="24">
-        <v>0</v>
-      </c>
-      <c r="M12" s="24">
+      <c r="O12" s="24">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24">
         <v>-5</v>
       </c>
-      <c r="N12" s="24">
-        <v>-10</v>
-      </c>
-      <c r="O12" s="24">
-        <v>0</v>
-      </c>
-      <c r="P12" s="24">
+      <c r="Q12" s="24">
+        <v>-10</v>
+      </c>
+      <c r="R12" s="24">
+        <v>0</v>
+      </c>
+      <c r="S12" s="24">
         <v>15</v>
       </c>
-      <c r="Q12" s="24">
-        <v>0</v>
-      </c>
-      <c r="R12" s="24">
+      <c r="T12" s="24">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24">
         <v>-5</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>1103</v>
       </c>
@@ -1646,38 +1753,47 @@
       <c r="H13" s="4">
         <v>0</v>
       </c>
-      <c r="I13" s="24">
-        <v>0</v>
-      </c>
-      <c r="J13" s="24">
-        <v>10</v>
-      </c>
-      <c r="K13" s="24">
-        <v>-10</v>
+      <c r="I13" s="4">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4">
+        <v>0</v>
+      </c>
+      <c r="K13" s="4">
+        <v>0</v>
       </c>
       <c r="L13" s="24">
         <v>0</v>
       </c>
       <c r="M13" s="24">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N13" s="24">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="O13" s="24">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="P13" s="24">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="24">
+        <v>0</v>
+      </c>
+      <c r="R13" s="24">
+        <v>-10</v>
+      </c>
+      <c r="S13" s="24">
         <v>15</v>
       </c>
-      <c r="Q13" s="24">
-        <v>-10</v>
-      </c>
-      <c r="R13" s="24">
+      <c r="T13" s="24">
+        <v>-10</v>
+      </c>
+      <c r="U13" s="24">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" s="16" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>3</v>
       </c>
@@ -1688,41 +1804,32 @@
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15">
-        <f>SUM(I14:M14)</f>
+        <f>SUM(L14:P14)</f>
         <v>15</v>
       </c>
       <c r="G14" s="15">
-        <f>SUM(N14:R14)</f>
+        <f>SUM(Q14:U14)</f>
         <v>20</v>
       </c>
       <c r="H14" s="14"/>
-      <c r="I14" s="14">
-        <f>SUM(I15:I18)</f>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14">
+        <f>SUM(L15:L18)</f>
         <v>20</v>
       </c>
-      <c r="J14" s="14">
-        <f t="shared" ref="J14:R14" si="2">SUM(J15:J18)</f>
+      <c r="M14" s="14">
+        <f t="shared" ref="M14:U14" si="2">SUM(M15:M18)</f>
         <v>-15</v>
       </c>
-      <c r="K14" s="14">
+      <c r="N14" s="14">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="L14" s="14">
+      <c r="O14" s="14">
         <f t="shared" si="2"/>
         <v>15</v>
-      </c>
-      <c r="M14" s="14">
-        <f t="shared" si="2"/>
-        <v>-15</v>
-      </c>
-      <c r="N14" s="14">
-        <f t="shared" si="2"/>
-        <v>-15</v>
-      </c>
-      <c r="O14" s="14">
-        <f t="shared" si="2"/>
-        <v>55</v>
       </c>
       <c r="P14" s="14">
         <f t="shared" si="2"/>
@@ -1730,14 +1837,26 @@
       </c>
       <c r="Q14" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-15</v>
       </c>
       <c r="R14" s="14">
         <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="S14" s="14">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+      <c r="T14" s="14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U14" s="14">
+        <f t="shared" si="2"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>1200</v>
       </c>
@@ -1762,38 +1881,47 @@
       <c r="H15" s="4">
         <v>0</v>
       </c>
-      <c r="I15" s="25">
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="25">
         <v>5</v>
       </c>
-      <c r="J15" s="25">
-        <v>-10</v>
-      </c>
-      <c r="K15" s="25">
-        <v>0</v>
-      </c>
-      <c r="L15" s="25">
+      <c r="M15" s="25">
+        <v>-10</v>
+      </c>
+      <c r="N15" s="25">
+        <v>0</v>
+      </c>
+      <c r="O15" s="25">
         <v>-5</v>
       </c>
-      <c r="M15" s="25">
-        <v>0</v>
-      </c>
-      <c r="N15" s="25">
+      <c r="P15" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="25">
         <v>-5</v>
       </c>
-      <c r="O15" s="25">
-        <v>10</v>
-      </c>
-      <c r="P15" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="25">
+      <c r="R15" s="25">
+        <v>10</v>
+      </c>
+      <c r="S15" s="25">
+        <v>0</v>
+      </c>
+      <c r="T15" s="25">
         <v>5</v>
       </c>
-      <c r="R15" s="25">
+      <c r="U15" s="25">
         <v>-10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>1201</v>
       </c>
@@ -1818,38 +1946,47 @@
       <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="I16" s="25">
+      <c r="I16" s="4">
+        <v>0</v>
+      </c>
+      <c r="J16" s="4">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0</v>
+      </c>
+      <c r="L16" s="25">
         <v>5</v>
       </c>
-      <c r="J16" s="25">
-        <v>-10</v>
-      </c>
-      <c r="K16" s="25">
-        <v>0</v>
-      </c>
-      <c r="L16" s="25">
-        <v>10</v>
-      </c>
       <c r="M16" s="25">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="N16" s="25">
+        <v>0</v>
+      </c>
+      <c r="O16" s="25">
+        <v>10</v>
+      </c>
+      <c r="P16" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="25">
         <v>-5</v>
       </c>
-      <c r="O16" s="25">
+      <c r="R16" s="25">
         <v>15</v>
       </c>
-      <c r="P16" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="25">
-        <v>-10</v>
-      </c>
-      <c r="R16" s="25">
+      <c r="S16" s="25">
+        <v>0</v>
+      </c>
+      <c r="T16" s="25">
+        <v>-10</v>
+      </c>
+      <c r="U16" s="25">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>1202</v>
       </c>
@@ -1874,38 +2011,47 @@
       <c r="H17" s="4">
         <v>0</v>
       </c>
-      <c r="I17" s="25">
-        <v>0</v>
-      </c>
-      <c r="J17" s="25">
-        <v>-10</v>
-      </c>
-      <c r="K17" s="25">
-        <v>10</v>
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
       </c>
       <c r="L17" s="25">
         <v>0</v>
       </c>
       <c r="M17" s="25">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="N17" s="25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="O17" s="25">
+        <v>0</v>
+      </c>
+      <c r="P17" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="25">
+        <v>0</v>
+      </c>
+      <c r="R17" s="25">
         <v>15</v>
       </c>
-      <c r="P17" s="25">
+      <c r="S17" s="25">
         <v>-15</v>
       </c>
-      <c r="Q17" s="25">
-        <v>0</v>
-      </c>
-      <c r="R17" s="25">
+      <c r="T17" s="25">
+        <v>0</v>
+      </c>
+      <c r="U17" s="25">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>1203</v>
       </c>
@@ -1930,38 +2076,47 @@
       <c r="H18" s="4">
         <v>0</v>
       </c>
-      <c r="I18" s="25">
-        <v>10</v>
-      </c>
-      <c r="J18" s="25">
+      <c r="I18" s="4">
+        <v>0</v>
+      </c>
+      <c r="J18" s="4">
+        <v>0</v>
+      </c>
+      <c r="K18" s="4">
+        <v>0</v>
+      </c>
+      <c r="L18" s="25">
+        <v>10</v>
+      </c>
+      <c r="M18" s="25">
         <v>15</v>
       </c>
-      <c r="K18" s="25">
-        <v>0</v>
-      </c>
-      <c r="L18" s="25">
-        <v>10</v>
-      </c>
-      <c r="M18" s="25">
+      <c r="N18" s="25">
+        <v>0</v>
+      </c>
+      <c r="O18" s="25">
+        <v>10</v>
+      </c>
+      <c r="P18" s="25">
         <v>-15</v>
       </c>
-      <c r="N18" s="25">
+      <c r="Q18" s="25">
         <v>-5</v>
       </c>
-      <c r="O18" s="25">
+      <c r="R18" s="25">
         <v>15</v>
       </c>
-      <c r="P18" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="25">
+      <c r="S18" s="25">
+        <v>0</v>
+      </c>
+      <c r="T18" s="25">
         <v>5</v>
       </c>
-      <c r="R18" s="25">
+      <c r="U18" s="25">
         <v>-5</v>
       </c>
     </row>
-    <row r="19" spans="1:18" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" s="22" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>3</v>
       </c>
@@ -1972,56 +2127,59 @@
       <c r="D19" s="20"/>
       <c r="E19" s="21"/>
       <c r="F19" s="23">
-        <f>SUM(I19:M19)</f>
+        <f>SUM(L19:P19)</f>
         <v>-10</v>
       </c>
       <c r="G19" s="23">
-        <f>SUM(N19:R19)</f>
+        <f>SUM(Q19:U19)</f>
         <v>-5</v>
       </c>
       <c r="H19" s="20"/>
-      <c r="I19" s="20">
-        <f>SUM(I20:I25)</f>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+      <c r="L19" s="20">
+        <f>SUM(L20:L25)</f>
         <v>15</v>
       </c>
-      <c r="J19" s="20">
-        <f t="shared" ref="J19:R19" si="3">SUM(J20:J25)</f>
-        <v>-10</v>
-      </c>
-      <c r="K19" s="20">
+      <c r="M19" s="20">
+        <f t="shared" ref="M19:U19" si="3">SUM(M20:M25)</f>
+        <v>-10</v>
+      </c>
+      <c r="N19" s="20">
         <f t="shared" si="3"/>
         <v>-10</v>
       </c>
-      <c r="L19" s="20">
+      <c r="O19" s="20">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="M19" s="20">
+      <c r="P19" s="20">
         <f t="shared" si="3"/>
         <v>-15</v>
       </c>
-      <c r="N19" s="20">
+      <c r="Q19" s="20">
         <f t="shared" si="3"/>
         <v>-10</v>
       </c>
-      <c r="O19" s="20">
+      <c r="R19" s="20">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="P19" s="20">
+      <c r="S19" s="20">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="T19" s="20">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="R19" s="20">
+      <c r="U19" s="20">
         <f t="shared" si="3"/>
         <v>-50</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>1300</v>
       </c>
@@ -2046,13 +2204,13 @@
       <c r="H20" s="4">
         <v>0</v>
       </c>
-      <c r="I20" s="25">
-        <v>0</v>
-      </c>
-      <c r="J20" s="25">
-        <v>0</v>
-      </c>
-      <c r="K20" s="25">
+      <c r="I20" s="4">
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>0</v>
+      </c>
+      <c r="K20" s="4">
         <v>0</v>
       </c>
       <c r="L20" s="25">
@@ -2062,22 +2220,31 @@
         <v>0</v>
       </c>
       <c r="N20" s="25">
+        <v>0</v>
+      </c>
+      <c r="O20" s="25">
+        <v>0</v>
+      </c>
+      <c r="P20" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="25">
         <v>-5</v>
       </c>
-      <c r="O20" s="25">
-        <v>0</v>
-      </c>
-      <c r="P20" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="25">
+      <c r="R20" s="25">
+        <v>0</v>
+      </c>
+      <c r="S20" s="25">
+        <v>0</v>
+      </c>
+      <c r="T20" s="25">
         <v>5</v>
       </c>
-      <c r="R20" s="25">
+      <c r="U20" s="25">
         <v>-5</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>1301</v>
       </c>
@@ -2102,38 +2269,47 @@
       <c r="H21" s="4">
         <v>0</v>
       </c>
-      <c r="I21" s="25">
+      <c r="I21" s="4">
+        <v>0</v>
+      </c>
+      <c r="J21" s="4">
+        <v>0</v>
+      </c>
+      <c r="K21" s="4">
+        <v>0</v>
+      </c>
+      <c r="L21" s="25">
         <v>5</v>
       </c>
-      <c r="J21" s="25">
-        <v>-10</v>
-      </c>
-      <c r="K21" s="25">
-        <v>0</v>
-      </c>
-      <c r="L21" s="25">
+      <c r="M21" s="25">
+        <v>-10</v>
+      </c>
+      <c r="N21" s="25">
+        <v>0</v>
+      </c>
+      <c r="O21" s="25">
         <v>15</v>
       </c>
-      <c r="M21" s="25">
-        <v>0</v>
-      </c>
-      <c r="N21" s="25">
+      <c r="P21" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="25">
         <v>5</v>
       </c>
-      <c r="O21" s="25">
-        <v>0</v>
-      </c>
-      <c r="P21" s="25">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="25">
-        <v>10</v>
-      </c>
       <c r="R21" s="25">
+        <v>0</v>
+      </c>
+      <c r="S21" s="25">
+        <v>0</v>
+      </c>
+      <c r="T21" s="25">
+        <v>10</v>
+      </c>
+      <c r="U21" s="25">
         <v>-10</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>1302</v>
       </c>
@@ -2158,13 +2334,13 @@
       <c r="H22" s="4">
         <v>0</v>
       </c>
-      <c r="I22" s="25">
-        <v>0</v>
-      </c>
-      <c r="J22" s="25">
-        <v>0</v>
-      </c>
-      <c r="K22" s="25">
+      <c r="I22" s="4">
+        <v>0</v>
+      </c>
+      <c r="J22" s="4">
+        <v>0</v>
+      </c>
+      <c r="K22" s="4">
         <v>0</v>
       </c>
       <c r="L22" s="25">
@@ -2183,13 +2359,22 @@
         <v>0</v>
       </c>
       <c r="Q22" s="25">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="R22" s="25">
+        <v>0</v>
+      </c>
+      <c r="S22" s="25">
+        <v>0</v>
+      </c>
+      <c r="T22" s="25">
+        <v>10</v>
+      </c>
+      <c r="U22" s="25">
         <v>-15</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>1303</v>
       </c>
@@ -2214,38 +2399,47 @@
       <c r="H23" s="4">
         <v>0</v>
       </c>
-      <c r="I23" s="25">
-        <v>0</v>
-      </c>
-      <c r="J23" s="25">
-        <v>0</v>
-      </c>
-      <c r="K23" s="25">
-        <v>-10</v>
+      <c r="I23" s="4">
+        <v>0</v>
+      </c>
+      <c r="J23" s="4">
+        <v>0</v>
+      </c>
+      <c r="K23" s="4">
+        <v>0</v>
       </c>
       <c r="L23" s="25">
         <v>0</v>
       </c>
       <c r="M23" s="25">
+        <v>0</v>
+      </c>
+      <c r="N23" s="25">
+        <v>-10</v>
+      </c>
+      <c r="O23" s="25">
+        <v>0</v>
+      </c>
+      <c r="P23" s="25">
         <v>-5</v>
       </c>
-      <c r="N23" s="25">
-        <v>0</v>
-      </c>
-      <c r="O23" s="25">
-        <v>0</v>
-      </c>
-      <c r="P23" s="25">
+      <c r="Q23" s="25">
+        <v>0</v>
+      </c>
+      <c r="R23" s="25">
+        <v>0</v>
+      </c>
+      <c r="S23" s="25">
         <v>15</v>
       </c>
-      <c r="Q23" s="25">
-        <v>-10</v>
-      </c>
-      <c r="R23" s="25">
+      <c r="T23" s="25">
+        <v>-10</v>
+      </c>
+      <c r="U23" s="25">
         <v>-5</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>1304</v>
       </c>
@@ -2270,38 +2464,47 @@
       <c r="H24" s="4">
         <v>0</v>
       </c>
-      <c r="I24" s="25">
-        <v>0</v>
-      </c>
-      <c r="J24" s="25">
-        <v>0</v>
-      </c>
-      <c r="K24" s="25">
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
         <v>0</v>
       </c>
       <c r="L24" s="25">
+        <v>0</v>
+      </c>
+      <c r="M24" s="25">
+        <v>0</v>
+      </c>
+      <c r="N24" s="25">
+        <v>0</v>
+      </c>
+      <c r="O24" s="25">
         <v>-15</v>
       </c>
-      <c r="M24" s="25">
-        <v>0</v>
-      </c>
-      <c r="N24" s="25">
-        <v>0</v>
-      </c>
-      <c r="O24" s="25">
-        <v>0</v>
-      </c>
       <c r="P24" s="25">
         <v>0</v>
       </c>
       <c r="Q24" s="25">
+        <v>0</v>
+      </c>
+      <c r="R24" s="25">
+        <v>0</v>
+      </c>
+      <c r="S24" s="25">
+        <v>0</v>
+      </c>
+      <c r="T24" s="25">
         <v>15</v>
       </c>
-      <c r="R24" s="25">
+      <c r="U24" s="25">
         <v>-15</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>1305</v>
       </c>
@@ -2326,38 +2529,47 @@
       <c r="H25" s="4">
         <v>0</v>
       </c>
-      <c r="I25" s="25">
-        <v>10</v>
-      </c>
-      <c r="J25" s="25">
-        <v>0</v>
-      </c>
-      <c r="K25" s="25">
+      <c r="I25" s="4">
+        <v>0</v>
+      </c>
+      <c r="J25" s="4">
+        <v>0</v>
+      </c>
+      <c r="K25" s="4">
         <v>0</v>
       </c>
       <c r="L25" s="25">
         <v>10</v>
       </c>
       <c r="M25" s="25">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="N25" s="25">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="O25" s="25">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="P25" s="25">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="Q25" s="25">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="R25" s="25">
         <v>0</v>
       </c>
+      <c r="S25" s="25">
+        <v>0</v>
+      </c>
+      <c r="T25" s="25">
+        <v>10</v>
+      </c>
+      <c r="U25" s="25">
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:18" s="28" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" s="28" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="26" t="s">
         <v>3</v>
       </c>
@@ -2368,41 +2580,32 @@
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27">
-        <f>SUM(I26:M26)</f>
+        <f>SUM(L26:P26)</f>
         <v>15</v>
       </c>
       <c r="G26" s="27">
-        <f>SUM(N26:R26)</f>
+        <f>SUM(Q26:U26)</f>
         <v>20</v>
       </c>
       <c r="H26" s="26"/>
-      <c r="I26" s="26">
-        <f>SUM(I27:I29)</f>
-        <v>10</v>
-      </c>
-      <c r="J26" s="26">
-        <f t="shared" ref="J26:R26" si="4">SUM(J27:J29)</f>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+      <c r="K26" s="26"/>
+      <c r="L26" s="26">
+        <f>SUM(L27:L29)</f>
+        <v>10</v>
+      </c>
+      <c r="M26" s="26">
+        <f t="shared" ref="M26:U26" si="4">SUM(M27:M29)</f>
         <v>5</v>
-      </c>
-      <c r="K26" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L26" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M26" s="26">
-        <f t="shared" si="4"/>
-        <v>0</v>
       </c>
       <c r="N26" s="26">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O26" s="26">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="P26" s="26">
         <f t="shared" si="4"/>
@@ -2410,14 +2613,26 @@
       </c>
       <c r="Q26" s="26">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R26" s="26">
         <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="S26" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T26" s="26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="U26" s="26">
+        <f t="shared" si="4"/>
         <v>-15</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>2000</v>
       </c>
@@ -2446,7 +2661,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K27" s="4">
         <v>0</v>
@@ -2455,13 +2670,13 @@
         <v>0</v>
       </c>
       <c r="M27" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N27" s="4">
         <v>0</v>
       </c>
       <c r="O27" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P27" s="4">
         <v>0</v>
@@ -2470,10 +2685,19 @@
         <v>0</v>
       </c>
       <c r="R27" s="4">
+        <v>10</v>
+      </c>
+      <c r="S27" s="4">
+        <v>0</v>
+      </c>
+      <c r="T27" s="4">
+        <v>0</v>
+      </c>
+      <c r="U27" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" ht="51" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>2001</v>
       </c>
@@ -2496,13 +2720,13 @@
         <v>98</v>
       </c>
       <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
         <v>2002</v>
       </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
       <c r="J28" s="4">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="K28" s="4">
         <v>0</v>
@@ -2511,13 +2735,13 @@
         <v>0</v>
       </c>
       <c r="M28" s="4">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="N28" s="4">
         <v>0</v>
       </c>
       <c r="O28" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="P28" s="4">
         <v>0</v>
@@ -2526,10 +2750,19 @@
         <v>0</v>
       </c>
       <c r="R28" s="4">
+        <v>10</v>
+      </c>
+      <c r="S28" s="4">
+        <v>0</v>
+      </c>
+      <c r="T28" s="4">
+        <v>0</v>
+      </c>
+      <c r="U28" s="4">
         <v>-15</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>2002</v>
       </c>
@@ -2555,38 +2788,47 @@
         <v>0</v>
       </c>
       <c r="I29" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J29" s="4">
+        <v>0</v>
+      </c>
+      <c r="K29" s="4">
+        <v>0</v>
+      </c>
+      <c r="L29" s="4">
+        <v>10</v>
+      </c>
+      <c r="M29" s="4">
         <v>5</v>
       </c>
-      <c r="K29" s="4">
-        <v>0</v>
-      </c>
-      <c r="L29" s="4">
-        <v>0</v>
-      </c>
-      <c r="M29" s="4">
-        <v>0</v>
-      </c>
       <c r="N29" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="O29" s="4">
+        <v>0</v>
+      </c>
+      <c r="P29" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="4">
+        <v>10</v>
+      </c>
+      <c r="R29" s="4">
         <v>5</v>
       </c>
-      <c r="P29" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="4">
-        <v>0</v>
-      </c>
-      <c r="R29" s="4">
+      <c r="S29" s="4">
+        <v>0</v>
+      </c>
+      <c r="T29" s="4">
+        <v>0</v>
+      </c>
+      <c r="U29" s="4">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I3:R8">
+  <conditionalFormatting sqref="L3:U8">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2598,7 +2840,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I10:R13">
+  <conditionalFormatting sqref="L10:U13">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2610,7 +2852,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I15:R18">
+  <conditionalFormatting sqref="L15:U18">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2622,7 +2864,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:R25">
+  <conditionalFormatting sqref="L20:U25">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2634,7 +2876,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I27:R29">
+  <conditionalFormatting sqref="L27:U29">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>